<commit_message>
Update SSP-Training to SSP 2.6 Patches
</commit_message>
<xml_diff>
--- a/SSP_TRAINING_DEFAULT_LOGIN_DATA.xlsx
+++ b/SSP_TRAINING_DEFAULT_LOGIN_DATA.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t>SSP Training Login and External Sync Information</t>
   </si>
@@ -82,12 +82,18 @@
     <t>rmiller342</t>
   </si>
   <si>
+    <t>faculty4</t>
+  </si>
+  <si>
     <t>ptaylor14</t>
   </si>
   <si>
     <t>probinson343</t>
   </si>
   <si>
+    <t>faculty5</t>
+  </si>
+  <si>
     <t>rmartinez11</t>
   </si>
   <si>
@@ -103,18 +109,27 @@
     <t>tdavis4</t>
   </si>
   <si>
+    <t>Manager Username</t>
+  </si>
+  <si>
     <t>pdavis13</t>
   </si>
   <si>
     <t>mtaylor5</t>
   </si>
   <si>
+    <t>manager1</t>
+  </si>
+  <si>
     <t>jjackson10</t>
   </si>
   <si>
     <t>rdavis50</t>
   </si>
   <si>
+    <t>manager2</t>
+  </si>
+  <si>
     <t>coach4</t>
   </si>
   <si>
@@ -124,18 +139,27 @@
     <t>mbrown51</t>
   </si>
   <si>
+    <t>manager3</t>
+  </si>
+  <si>
     <t>lwhite112</t>
   </si>
   <si>
     <t>pthompson326</t>
   </si>
   <si>
+    <t>manager4</t>
+  </si>
+  <si>
     <t>mrodriguez17</t>
   </si>
   <si>
     <t>cjackson52</t>
   </si>
   <si>
+    <t>manager5</t>
+  </si>
+  <si>
     <t>coach5</t>
   </si>
   <si>
@@ -151,12 +175,18 @@
     <t>swhite53</t>
   </si>
   <si>
+    <t>Support Staff Username</t>
+  </si>
+  <si>
     <t>jmartinez110</t>
   </si>
   <si>
     <t>janderson56</t>
   </si>
   <si>
+    <t>supportstaff1</t>
+  </si>
+  <si>
     <t>coach6</t>
   </si>
   <si>
@@ -166,18 +196,27 @@
     <t>jtaylor57</t>
   </si>
   <si>
+    <t>supportstaff2</t>
+  </si>
+  <si>
     <t>sthomas20</t>
   </si>
   <si>
     <t>landerson313</t>
   </si>
   <si>
+    <t>supportstaff3</t>
+  </si>
+  <si>
     <t>manderson16</t>
   </si>
   <si>
     <t>cwilson598</t>
   </si>
   <si>
+    <t>supportstaff4</t>
+  </si>
+  <si>
     <t>coach7</t>
   </si>
   <si>
@@ -187,6 +226,9 @@
     <t>mbrown511</t>
   </si>
   <si>
+    <t>supportstaff5</t>
+  </si>
+  <si>
     <t>jdavis24</t>
   </si>
   <si>
@@ -199,6 +241,9 @@
     <t>rmartin512</t>
   </si>
   <si>
+    <t>Developer Username</t>
+  </si>
+  <si>
     <t>coach8</t>
   </si>
   <si>
@@ -206,6 +251,9 @@
   </si>
   <si>
     <t>rtaylor514</t>
+  </si>
+  <si>
+    <t>developer1</t>
   </si>
   <si>
     <t>mdavis25</t>
@@ -434,9 +482,10 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -457,18 +506,28 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="14"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="14"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
       <sz val="12"/>
     </font>
     <font>
@@ -544,73 +603,73 @@
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
+      <left style="medium"/>
       <right style="hair"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
       <left style="hair"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
+      <left style="medium"/>
       <right style="hair"/>
-      <top style="thin"/>
+      <top style="medium"/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
+      <left style="medium"/>
       <right style="hair"/>
       <top style="hair"/>
-      <bottom style="thin"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
+      <left style="medium"/>
+      <right style="medium"/>
       <top style="hair"/>
-      <bottom style="thin"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
+      <left style="medium"/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
+      <left style="medium"/>
+      <right style="medium"/>
       <top style="hair"/>
       <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
+      <left style="medium"/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
   </borders>
@@ -639,7 +698,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="4" numFmtId="164" xfId="0">
@@ -682,6 +741,9 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="7" fontId="6" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="5" fontId="8" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="8" fontId="0" numFmtId="164" xfId="0"/>
@@ -769,18 +831,18 @@
   <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E89" activeCellId="0" pane="topLeft" sqref="E89"/>
+      <selection activeCell="F34" activeCellId="0" pane="topLeft" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.8078431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.0509803921569"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.521568627451"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="2.50588235294118"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.6274509803922"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.9294117647059"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="3.06666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="1.81960784313725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.2588235294118"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.7450980392157"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="2.51372549019608"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.8274509803922"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.1294117647059"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="3.08235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="8.95" outlineLevel="0" r="1">
@@ -903,876 +965,908 @@
       <c r="E9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="10">
       <c r="A10" s="1"/>
       <c r="B10" s="13"/>
       <c r="C10" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="18"/>
+        <v>23</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>24</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="11">
       <c r="A11" s="1"/>
       <c r="B11" s="13"/>
       <c r="C11" s="14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="18"/>
+        <v>26</v>
+      </c>
+      <c r="F11" s="19"/>
       <c r="G11" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="12">
       <c r="A12" s="1"/>
       <c r="B12" s="9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="18"/>
+        <v>29</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="13">
       <c r="A13" s="1"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="18"/>
+        <v>32</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>33</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="14">
       <c r="A14" s="1"/>
       <c r="B14" s="13"/>
       <c r="C14" s="14" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="18"/>
+        <v>35</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>36</v>
+      </c>
       <c r="G14" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="15">
       <c r="A15" s="1"/>
       <c r="B15" s="9" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="18"/>
+        <v>39</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>40</v>
+      </c>
       <c r="G15" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="16">
       <c r="A16" s="1"/>
       <c r="B16" s="13"/>
       <c r="C16" s="14" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="18"/>
+        <v>42</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>43</v>
+      </c>
       <c r="G16" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="17">
       <c r="A17" s="1"/>
       <c r="B17" s="13"/>
       <c r="C17" s="14" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="18"/>
+        <v>45</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>46</v>
+      </c>
       <c r="G17" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="18">
       <c r="A18" s="1"/>
       <c r="B18" s="9" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="18"/>
+        <v>49</v>
+      </c>
+      <c r="F18" s="19"/>
       <c r="G18" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="19">
       <c r="A19" s="1"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" s="18"/>
+        <v>51</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="G19" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="20">
       <c r="A20" s="1"/>
       <c r="B20" s="13"/>
       <c r="C20" s="14" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="18"/>
+        <v>54</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="G20" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="21">
       <c r="A21" s="1"/>
       <c r="B21" s="9" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="18"/>
+        <v>58</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>59</v>
+      </c>
       <c r="G21" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="22">
       <c r="A22" s="1"/>
       <c r="B22" s="13"/>
       <c r="C22" s="14" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="18"/>
+        <v>61</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="G22" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="23">
       <c r="A23" s="1"/>
       <c r="B23" s="13"/>
       <c r="C23" s="14" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="18"/>
+        <v>64</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>65</v>
+      </c>
       <c r="G23" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="24">
       <c r="A24" s="1"/>
       <c r="B24" s="9" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" s="18"/>
+        <v>68</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>69</v>
+      </c>
       <c r="G24" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="25">
       <c r="A25" s="1"/>
       <c r="B25" s="13"/>
       <c r="C25" s="14" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F25" s="18"/>
+        <v>71</v>
+      </c>
+      <c r="F25" s="19"/>
       <c r="G25" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="26">
       <c r="A26" s="1"/>
       <c r="B26" s="13"/>
       <c r="C26" s="14" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" s="18"/>
+        <v>73</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>74</v>
+      </c>
       <c r="G26" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="27">
       <c r="A27" s="1"/>
       <c r="B27" s="9" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="18"/>
+        <v>77</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>78</v>
+      </c>
       <c r="G27" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="28">
       <c r="A28" s="1"/>
       <c r="B28" s="13"/>
       <c r="C28" s="14" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="18"/>
+        <v>80</v>
+      </c>
+      <c r="F28" s="19"/>
       <c r="G28" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="29">
       <c r="A29" s="1"/>
       <c r="B29" s="13"/>
       <c r="C29" s="14" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="18"/>
+        <v>82</v>
+      </c>
+      <c r="F29" s="19"/>
       <c r="G29" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="30">
       <c r="A30" s="1"/>
       <c r="B30" s="9" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="F30" s="18"/>
+        <v>85</v>
+      </c>
+      <c r="F30" s="19"/>
       <c r="G30" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="31">
       <c r="A31" s="1"/>
       <c r="B31" s="13"/>
       <c r="C31" s="14" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D31" s="1"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
       <c r="G31" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="32">
       <c r="A32" s="1"/>
       <c r="B32" s="13"/>
       <c r="C32" s="14" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
       <c r="G32" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="33">
       <c r="A33" s="1"/>
       <c r="B33" s="9" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="D33" s="1"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
       <c r="G33" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="34">
       <c r="A34" s="1"/>
       <c r="B34" s="13"/>
       <c r="C34" s="14" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="D34" s="1"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
       <c r="G34" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="35">
       <c r="A35" s="1"/>
       <c r="B35" s="13"/>
       <c r="C35" s="14" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="D35" s="1"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
       <c r="G35" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="36">
       <c r="A36" s="1"/>
       <c r="B36" s="9" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
       <c r="G36" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="37">
       <c r="A37" s="1"/>
       <c r="B37" s="13"/>
       <c r="C37" s="14" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="D37" s="1"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
       <c r="G37" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="38">
       <c r="A38" s="1"/>
       <c r="B38" s="13"/>
       <c r="C38" s="14" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
       <c r="G38" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="39">
       <c r="A39" s="1"/>
       <c r="B39" s="9" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="D39" s="1"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
       <c r="G39" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="40">
       <c r="A40" s="1"/>
       <c r="B40" s="13"/>
       <c r="C40" s="14" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D40" s="1"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
       <c r="G40" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="41">
       <c r="A41" s="1"/>
       <c r="B41" s="13"/>
       <c r="C41" s="14" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="D41" s="1"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
       <c r="G41" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="42">
       <c r="A42" s="1"/>
       <c r="B42" s="9" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="D42" s="1"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
       <c r="G42" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="43">
       <c r="A43" s="1"/>
       <c r="B43" s="13"/>
       <c r="C43" s="14" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="D43" s="1"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
       <c r="G43" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="44">
       <c r="A44" s="1"/>
       <c r="B44" s="13"/>
       <c r="C44" s="14" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="D44" s="1"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
       <c r="G44" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="45">
       <c r="A45" s="1"/>
       <c r="B45" s="9" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="D45" s="1"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
       <c r="G45" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="46">
       <c r="A46" s="1"/>
       <c r="B46" s="13"/>
       <c r="C46" s="14" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="D46" s="1"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
       <c r="G46" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="47">
       <c r="A47" s="1"/>
       <c r="B47" s="13"/>
       <c r="C47" s="14" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="D47" s="1"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
       <c r="G47" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="48">
       <c r="A48" s="1"/>
       <c r="B48" s="9" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="D48" s="1"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
       <c r="G48" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="49">
       <c r="A49" s="1"/>
       <c r="B49" s="13"/>
       <c r="C49" s="14" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="D49" s="1"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
       <c r="G49" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="50">
       <c r="A50" s="1"/>
       <c r="B50" s="13"/>
       <c r="C50" s="14" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="D50" s="1"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
       <c r="G50" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="51">
       <c r="A51" s="1"/>
       <c r="B51" s="9" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D51" s="1"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
       <c r="G51" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="52">
       <c r="A52" s="1"/>
       <c r="B52" s="13"/>
       <c r="C52" s="14" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="D52" s="1"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
       <c r="G52" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="53">
       <c r="A53" s="1"/>
       <c r="B53" s="13"/>
       <c r="C53" s="14" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="D53" s="1"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
       <c r="G53" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="54">
       <c r="A54" s="1"/>
       <c r="B54" s="9" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="D54" s="1"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
       <c r="G54" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="55">
       <c r="A55" s="1"/>
       <c r="B55" s="13"/>
       <c r="C55" s="14" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="D55" s="1"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
       <c r="G55" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="56">
       <c r="A56" s="1"/>
       <c r="B56" s="13"/>
       <c r="C56" s="14" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="D56" s="1"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
       <c r="G56" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="57">
       <c r="A57" s="1"/>
       <c r="B57" s="9" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="D57" s="1"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
       <c r="G57" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="58">
       <c r="A58" s="1"/>
       <c r="B58" s="13"/>
       <c r="C58" s="14" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="D58" s="1"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
       <c r="G58" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="59">
       <c r="A59" s="1"/>
       <c r="B59" s="13"/>
       <c r="C59" s="14" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="D59" s="1"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
       <c r="G59" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="60">
       <c r="A60" s="1"/>
       <c r="B60" s="9" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="D60" s="1"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
       <c r="G60" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="61">
       <c r="A61" s="1"/>
       <c r="B61" s="13"/>
       <c r="C61" s="14" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="D61" s="1"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
       <c r="G61" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="62">
       <c r="A62" s="1"/>
       <c r="B62" s="13"/>
       <c r="C62" s="14" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="D62" s="1"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
       <c r="G62" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="63">
       <c r="A63" s="1"/>
       <c r="B63" s="9" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="D63" s="1"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
       <c r="G63" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="64">
       <c r="A64" s="1"/>
       <c r="B64" s="13"/>
       <c r="C64" s="14" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="D64" s="1"/>
-      <c r="E64" s="18"/>
-      <c r="F64" s="18"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
       <c r="G64" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="65">
       <c r="A65" s="1"/>
       <c r="B65" s="13"/>
       <c r="C65" s="14" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="D65" s="1"/>
-      <c r="E65" s="18"/>
-      <c r="F65" s="18"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
       <c r="G65" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="66">
       <c r="A66" s="1"/>
       <c r="B66" s="9" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="D66" s="1"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
       <c r="G66" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="67">
       <c r="A67" s="1"/>
       <c r="B67" s="13"/>
       <c r="C67" s="14" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D67" s="1"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="18"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
       <c r="G67" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="68">
       <c r="A68" s="1"/>
       <c r="B68" s="13"/>
       <c r="C68" s="14" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="D68" s="1"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="18"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
       <c r="G68" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="69">
       <c r="A69" s="1"/>
       <c r="B69" s="9" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="D69" s="1"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="18"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
       <c r="G69" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="70">
       <c r="A70" s="1"/>
       <c r="B70" s="13"/>
       <c r="C70" s="14" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D70" s="1"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="19"/>
       <c r="G70" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="71">
       <c r="A71" s="1"/>
       <c r="B71" s="13"/>
       <c r="C71" s="14" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="D71" s="1"/>
-      <c r="E71" s="18"/>
-      <c r="F71" s="18"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
       <c r="G71" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="72">
       <c r="A72" s="1"/>
       <c r="B72" s="9" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="D72" s="1"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="18"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
       <c r="G72" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="73">
       <c r="A73" s="1"/>
       <c r="B73" s="13"/>
       <c r="C73" s="14" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="D73" s="1"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="18"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
       <c r="G73" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="74">
       <c r="A74" s="1"/>
       <c r="B74" s="13"/>
       <c r="C74" s="14" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="D74" s="1"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
       <c r="G74" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="75">
       <c r="A75" s="1"/>
       <c r="B75" s="9" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="D75" s="1"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="18"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
       <c r="G75" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="76">
       <c r="A76" s="1"/>
       <c r="B76" s="13"/>
       <c r="C76" s="14" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="D76" s="1"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="18"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
       <c r="G76" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="77">
       <c r="A77" s="1"/>
       <c r="B77" s="13"/>
       <c r="C77" s="14" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="D77" s="1"/>
-      <c r="E77" s="18"/>
-      <c r="F77" s="18"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="19"/>
       <c r="G77" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="78">
       <c r="A78" s="1"/>
       <c r="B78" s="9" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="D78" s="1"/>
-      <c r="E78" s="18"/>
-      <c r="F78" s="18"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="19"/>
       <c r="G78" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="79">
       <c r="A79" s="1"/>
       <c r="B79" s="13"/>
       <c r="C79" s="14" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="D79" s="1"/>
-      <c r="E79" s="18"/>
-      <c r="F79" s="18"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
       <c r="G79" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="25.2" outlineLevel="0" r="80">
       <c r="A80" s="1"/>
-      <c r="B80" s="19"/>
-      <c r="C80" s="20" t="s">
-        <v>135</v>
+      <c r="B80" s="20"/>
+      <c r="C80" s="21" t="s">
+        <v>151</v>
       </c>
       <c r="D80" s="1"/>
-      <c r="E80" s="18"/>
-      <c r="F80" s="18"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
       <c r="G80" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.15" outlineLevel="0" r="81">
@@ -1811,7 +1905,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1836,7 +1930,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>